<commit_message>
added grid view and some UI changes
</commit_message>
<xml_diff>
--- a/App/google_solution/Categories.xlsx
+++ b/App/google_solution/Categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_solutions\App\google_solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBFE279-D8B8-40E4-966D-5996B2353F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C07DE7-B56C-4540-9A47-385D4BEFE2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4656" yWindow="3228" windowWidth="17280" windowHeight="8964" xr2:uid="{0B0BE18B-0EB5-4F46-A727-E622F804091C}"/>
   </bookViews>
@@ -142,9 +142,6 @@
     <t>Pet Products</t>
   </si>
   <si>
-    <t>Baby Images</t>
-  </si>
-  <si>
     <t>https://hips.hearstapps.com/amv-prod-tpw.s3.amazonaws.com/wp-content/uploads/2016/02/pets_final2-2.jpg?resize=480:*</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>https://media.istockphoto.com/vectors/colorful-vector-cosmetic-bottles-set-flat-design-vector-id931012228?b=1&amp;k=20&amp;m=931012228&amp;s=612x612&amp;w=0&amp;h=U9yZjXWrvVD4MUcuJCDmt_5GdF_YE9Uytcft5sf3bRc=</t>
+  </si>
+  <si>
+    <t>Baby Products</t>
   </si>
 </sst>
 </file>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE005E-6271-4AF1-BCFC-E0074C22FF1E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -738,10 +738,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
COnnected firebase to the UI
</commit_message>
<xml_diff>
--- a/App/google_solution/Categories.xlsx
+++ b/App/google_solution/Categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google_solutions\App\google_solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C07DE7-B56C-4540-9A47-385D4BEFE2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBFE279-D8B8-40E4-966D-5996B2353F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4656" yWindow="3228" windowWidth="17280" windowHeight="8964" xr2:uid="{0B0BE18B-0EB5-4F46-A727-E622F804091C}"/>
   </bookViews>
@@ -142,6 +142,9 @@
     <t>Pet Products</t>
   </si>
   <si>
+    <t>Baby Images</t>
+  </si>
+  <si>
     <t>https://hips.hearstapps.com/amv-prod-tpw.s3.amazonaws.com/wp-content/uploads/2016/02/pets_final2-2.jpg?resize=480:*</t>
   </si>
   <si>
@@ -152,9 +155,6 @@
   </si>
   <si>
     <t>https://media.istockphoto.com/vectors/colorful-vector-cosmetic-bottles-set-flat-design-vector-id931012228?b=1&amp;k=20&amp;m=931012228&amp;s=612x612&amp;w=0&amp;h=U9yZjXWrvVD4MUcuJCDmt_5GdF_YE9Uytcft5sf3bRc=</t>
-  </si>
-  <si>
-    <t>Baby Products</t>
   </si>
 </sst>
 </file>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE005E-6271-4AF1-BCFC-E0074C22FF1E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -738,10 +738,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>